<commit_message>
Added new demo files
</commit_message>
<xml_diff>
--- a/XALINSClassFiles/Resources/CustomerData.xlsx
+++ b/XALINSClassFiles/Resources/CustomerData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\XALINS-Alteryx-Concepts-Level-1\XALINSClassFiles\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\XALINS-Alteryx-Concepts-Level-1\XALINSClassFiles\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F90B067-E257-437E-872B-B674DA58B0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,25 +184,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Customers" displayName="Customers" ref="A1:E11" totalsRowShown="0">
-  <autoFilter ref="A1:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Customers" displayName="Customers" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="CustomerID"/>
-    <tableColumn id="2" name="FirstName"/>
-    <tableColumn id="3" name="LastName"/>
-    <tableColumn id="4" name="CustomerCategory"/>
-    <tableColumn id="5" name="TotalSales"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CustomerID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FirstName"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LastName"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CustomerCategory"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TotalSales"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CustomerCategories" displayName="CustomerCategories" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CustomerCategories" displayName="CustomerCategories" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Category"/>
-    <tableColumn id="2" name="Discount" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Discount" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -469,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,10 +683,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>